<commit_message>
first iteration of implementing grouping
</commit_message>
<xml_diff>
--- a/data/electoral/Congressmen (version 1).xlsx
+++ b/data/electoral/Congressmen (version 1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="5520" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25520" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3551" uniqueCount="2605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3549" uniqueCount="2606">
   <si>
     <t>Alabama</t>
   </si>
@@ -19151,7 +19151,10 @@
     </r>
   </si>
   <si>
-    <t>Age</t>
+    <t>CurrentAge</t>
+  </si>
+  <si>
+    <t>John Kennedy</t>
   </si>
 </sst>
 </file>
@@ -19168,7 +19171,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -21043,10 +21045,10 @@
   <dimension ref="A1:Q109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="M1" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -22660,28 +22662,34 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="4" t="s">
-        <v>210</v>
+        <v>2605</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="D38" s="6"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
+      <c r="C38" s="6">
+        <v>18953</v>
+      </c>
+      <c r="D38" s="6">
+        <v>42738</v>
+      </c>
+      <c r="E38" s="4">
+        <v>65</v>
+      </c>
+      <c r="F38" s="4">
+        <v>43</v>
+      </c>
       <c r="G38" s="4">
         <v>0</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>210</v>
+        <v>225</v>
+      </c>
+      <c r="J38" s="13">
+        <v>65</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4">
@@ -22709,11 +22717,11 @@
         <v>41277</v>
       </c>
       <c r="E39" s="4">
-        <f>DATEDIF(C39,D39,"y")</f>
+        <f t="shared" ref="E39:E70" si="0">DATEDIF(C39,D39,"y")</f>
         <v>68</v>
       </c>
       <c r="F39" s="5">
-        <f>DATEDIF(C39,D39,"yd")</f>
+        <f t="shared" ref="F39:F70" si="1">DATEDIF(C39,D39,"yd")</f>
         <v>278</v>
       </c>
       <c r="G39" s="4">
@@ -22754,11 +22762,11 @@
         <v>35433</v>
       </c>
       <c r="E40" s="4">
-        <f t="shared" ref="E40:E103" si="0">DATEDIF(C40,D40,"y")</f>
+        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="F40" s="5">
-        <f t="shared" ref="F40:F103" si="1">DATEDIF(C40,D40,"yd")</f>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="G40" s="4">
@@ -24149,11 +24157,11 @@
         <v>36163</v>
       </c>
       <c r="E71" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E71:E102" si="2">DATEDIF(C71,D71,"y")</f>
         <v>48</v>
       </c>
       <c r="F71" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F71:F102" si="3">DATEDIF(C71,D71,"yd")</f>
         <v>41</v>
       </c>
       <c r="G71" s="4">
@@ -24194,11 +24202,11 @@
         <v>39839</v>
       </c>
       <c r="E72" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="F72" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>48</v>
       </c>
       <c r="G72" s="4">
@@ -24239,11 +24247,11 @@
         <v>38355</v>
       </c>
       <c r="E73" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="F73" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>34</v>
       </c>
       <c r="G73" s="4">
@@ -24284,11 +24292,11 @@
         <v>42007</v>
       </c>
       <c r="E74" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="F74" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>126</v>
       </c>
       <c r="G74" s="4">
@@ -24329,11 +24337,11 @@
         <v>41277</v>
       </c>
       <c r="E75" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="F75" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>308</v>
       </c>
       <c r="G75" s="4">
@@ -24374,11 +24382,11 @@
         <v>41277</v>
       </c>
       <c r="E76" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>57</v>
       </c>
       <c r="F76" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>65</v>
       </c>
       <c r="G76" s="4">
@@ -24419,11 +24427,11 @@
         <v>40546</v>
       </c>
       <c r="E77" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>53</v>
       </c>
       <c r="F77" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>296</v>
       </c>
       <c r="G77" s="4">
@@ -24464,11 +24472,11 @@
         <v>40546</v>
       </c>
       <c r="E78" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>55</v>
       </c>
       <c r="F78" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="G78" s="4">
@@ -24509,11 +24517,11 @@
         <v>39085</v>
       </c>
       <c r="E79" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="F79" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="G79" s="4">
@@ -24554,11 +24562,11 @@
         <v>42007</v>
       </c>
       <c r="E80" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="F80" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>305</v>
       </c>
       <c r="G80" s="4">
@@ -24599,11 +24607,11 @@
         <v>34655</v>
       </c>
       <c r="E81" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="F81" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G81" s="4">
@@ -24644,11 +24652,11 @@
         <v>39816</v>
       </c>
       <c r="E82" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="F82" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="G82" s="4">
@@ -24689,11 +24697,11 @@
         <v>35101</v>
       </c>
       <c r="E83" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="F83" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>279</v>
       </c>
       <c r="G83" s="4">
@@ -24734,11 +24742,11 @@
         <v>39085</v>
       </c>
       <c r="E84" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="F84" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>265</v>
       </c>
       <c r="G84" s="4">
@@ -24779,11 +24787,11 @@
         <v>40546</v>
       </c>
       <c r="E85" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>49</v>
       </c>
       <c r="F85" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47</v>
       </c>
       <c r="G85" s="4">
@@ -24824,11 +24832,11 @@
         <v>35433</v>
       </c>
       <c r="E86" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="F86" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>52</v>
       </c>
       <c r="G86" s="4">
@@ -24869,11 +24877,11 @@
         <v>39085</v>
       </c>
       <c r="E87" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>51</v>
       </c>
       <c r="F87" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>75</v>
       </c>
       <c r="G87" s="4">
@@ -24914,11 +24922,11 @@
         <v>37624</v>
       </c>
       <c r="E88" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="F88" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>178</v>
       </c>
       <c r="G88" s="4">
@@ -24959,11 +24967,11 @@
         <v>41276</v>
       </c>
       <c r="E89" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>47</v>
       </c>
       <c r="F89" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>105</v>
       </c>
       <c r="G89" s="4">
@@ -25004,11 +25012,11 @@
         <v>38355</v>
       </c>
       <c r="E90" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="F90" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>361</v>
       </c>
       <c r="G90" s="4">
@@ -25049,11 +25057,11 @@
         <v>42007</v>
       </c>
       <c r="E91" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="F91" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>71</v>
       </c>
       <c r="G91" s="4">
@@ -25094,11 +25102,11 @@
         <v>39085</v>
       </c>
       <c r="E92" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="F92" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>132</v>
       </c>
       <c r="G92" s="4">
@@ -25139,11 +25147,11 @@
         <v>37591</v>
       </c>
       <c r="E93" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="F93" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>303</v>
       </c>
       <c r="G93" s="4">
@@ -25184,11 +25192,11 @@
         <v>41277</v>
       </c>
       <c r="E94" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="F94" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G94" s="4">
@@ -25229,11 +25237,11 @@
         <v>40546</v>
       </c>
       <c r="E95" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="F95" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>213</v>
       </c>
       <c r="G95" s="4">
@@ -25274,11 +25282,11 @@
         <v>28128</v>
       </c>
       <c r="E96" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="F96" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>287</v>
       </c>
       <c r="G96" s="4">
@@ -25319,11 +25327,11 @@
         <v>39085</v>
       </c>
       <c r="E97" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>65</v>
       </c>
       <c r="F97" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>117</v>
       </c>
       <c r="G97" s="4">
@@ -25364,11 +25372,11 @@
         <v>27397</v>
       </c>
       <c r="E98" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>34</v>
       </c>
       <c r="F98" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>278</v>
       </c>
       <c r="G98" s="4">
@@ -25409,11 +25417,11 @@
         <v>39816</v>
       </c>
       <c r="E99" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="F99" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="G99" s="4">
@@ -25454,11 +25462,11 @@
         <v>41277</v>
       </c>
       <c r="E100" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>54</v>
       </c>
       <c r="F100" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>311</v>
       </c>
       <c r="G100" s="4">
@@ -25499,11 +25507,11 @@
         <v>36894</v>
       </c>
       <c r="E101" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="F101" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
       <c r="G101" s="4">
@@ -25544,11 +25552,11 @@
         <v>33972</v>
       </c>
       <c r="E102" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="F102" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>84</v>
       </c>
       <c r="G102" s="4">
@@ -25589,11 +25597,11 @@
         <v>40497</v>
       </c>
       <c r="E103" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E103:E134" si="4">DATEDIF(C103,D103,"y")</f>
         <v>63</v>
       </c>
       <c r="F103" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="F103:F108" si="5">DATEDIF(C103,D103,"yd")</f>
         <v>83</v>
       </c>
       <c r="G103" s="4">
@@ -25634,11 +25642,11 @@
         <v>42007</v>
       </c>
       <c r="E104" s="4">
-        <f t="shared" ref="E104:E108" si="2">DATEDIF(C104,D104,"y")</f>
+        <f t="shared" si="4"/>
         <v>61</v>
       </c>
       <c r="F104" s="5">
-        <f t="shared" ref="F104:F108" si="3">DATEDIF(C104,D104,"yd")</f>
+        <f t="shared" si="5"/>
         <v>38</v>
       </c>
       <c r="G104" s="4">
@@ -25679,11 +25687,11 @@
         <v>41277</v>
       </c>
       <c r="E105" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="F105" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>326</v>
       </c>
       <c r="G105" s="4">
@@ -25724,11 +25732,11 @@
         <v>40546</v>
       </c>
       <c r="E106" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>55</v>
       </c>
       <c r="F106" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>270</v>
       </c>
       <c r="G106" s="4">
@@ -25769,11 +25777,11 @@
         <v>39258</v>
       </c>
       <c r="E107" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>54</v>
       </c>
       <c r="F107" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>339</v>
       </c>
       <c r="G107" s="4">
@@ -25814,11 +25822,11 @@
         <v>35433</v>
       </c>
       <c r="E108" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>52</v>
       </c>
       <c r="F108" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>337</v>
       </c>
       <c r="G108" s="4">

</xml_diff>